<commit_message>
& - Актуализация - №71561403 от 10.10.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/Foreign_various/Foreighn_duplicates.xlsx
+++ b/Collections/Foreign_various/Foreighn_duplicates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\Foreign_various\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F61813-775D-4CA5-A7C5-2927B123CC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A86FC1-2731-4567-A943-F8A3A47783CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="106">
   <si>
     <t>-</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>50 копиек</t>
+  </si>
+  <si>
+    <t>1 тенге</t>
   </si>
 </sst>
 </file>
@@ -433,6 +436,8 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="6">
@@ -581,7 +586,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -641,6 +646,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -728,15 +736,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF9BE5FF"/>
@@ -935,6 +934,15 @@
           <bgColor rgb="FF9BE5FF"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -987,9 +995,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="7" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="32" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1258,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1272,41 +1280,41 @@
     <col min="7" max="9" width="12.36328125" customWidth="1"/>
     <col min="10" max="10" width="9.7265625" customWidth="1"/>
     <col min="11" max="12" width="11.1796875" customWidth="1"/>
-    <col min="13" max="32" width="8.7265625" customWidth="1"/>
+    <col min="13" max="31" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
@@ -1326,10 +1334,10 @@
       <c r="I2" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="26"/>
+      <c r="J2" s="27"/>
       <c r="K2" s="1"/>
-      <c r="O2">
-        <v>90</v>
+      <c r="O2" s="6">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1357,7 +1365,7 @@
       </c>
       <c r="I3" s="7">
         <f t="shared" ref="I3:I22" si="0">H3*$O$2</f>
-        <v>23.400000000000002</v>
+        <v>26</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>15</v>
@@ -1387,7 +1395,7 @@
       </c>
       <c r="I4" s="7">
         <f t="shared" si="0"/>
-        <v>56.7</v>
+        <v>63</v>
       </c>
       <c r="J4" s="18" t="s">
         <v>15</v>
@@ -1416,7 +1424,7 @@
       </c>
       <c r="I5" s="7">
         <f t="shared" si="0"/>
-        <v>84.6</v>
+        <v>94</v>
       </c>
       <c r="J5" s="18" t="s">
         <v>15</v>
@@ -1445,7 +1453,7 @@
       </c>
       <c r="I6" s="7">
         <f t="shared" si="0"/>
-        <v>99.000000000000014</v>
+        <v>110.00000000000001</v>
       </c>
       <c r="J6" s="18" t="s">
         <v>15</v>
@@ -1474,7 +1482,7 @@
       </c>
       <c r="I7" s="7">
         <f t="shared" si="0"/>
-        <v>95.4</v>
+        <v>106</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>15</v>
@@ -1503,7 +1511,7 @@
       </c>
       <c r="I8" s="7">
         <f t="shared" si="0"/>
-        <v>32.4</v>
+        <v>36</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>15</v>
@@ -1532,7 +1540,7 @@
       </c>
       <c r="I9" s="7">
         <f t="shared" si="0"/>
-        <v>44.1</v>
+        <v>49</v>
       </c>
       <c r="J9" s="18" t="s">
         <v>15</v>
@@ -1561,7 +1569,7 @@
       </c>
       <c r="I10" s="7">
         <f t="shared" si="0"/>
-        <v>102.6</v>
+        <v>113.99999999999999</v>
       </c>
       <c r="J10" s="18" t="s">
         <v>15</v>
@@ -1590,7 +1598,7 @@
       </c>
       <c r="I11" s="7">
         <f t="shared" si="0"/>
-        <v>35.1</v>
+        <v>39</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>15</v>
@@ -1619,7 +1627,7 @@
       </c>
       <c r="I12" s="7">
         <f t="shared" si="0"/>
-        <v>35.1</v>
+        <v>39</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>15</v>
@@ -1648,7 +1656,7 @@
       </c>
       <c r="I13" s="7">
         <f t="shared" si="0"/>
-        <v>11.700000000000001</v>
+        <v>13</v>
       </c>
       <c r="J13" s="18" t="s">
         <v>15</v>
@@ -1677,7 +1685,7 @@
       </c>
       <c r="I14" s="7">
         <f t="shared" si="0"/>
-        <v>14.4</v>
+        <v>16</v>
       </c>
       <c r="J14" s="18" t="s">
         <v>15</v>
@@ -1706,7 +1714,7 @@
       </c>
       <c r="I15" s="7">
         <f t="shared" si="0"/>
-        <v>19.8</v>
+        <v>22</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>15</v>
@@ -1735,7 +1743,7 @@
       </c>
       <c r="I16" s="7">
         <f t="shared" si="0"/>
-        <v>19.8</v>
+        <v>22</v>
       </c>
       <c r="J16" s="18" t="s">
         <v>15</v>
@@ -1764,7 +1772,7 @@
       </c>
       <c r="I17" s="7">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J17" s="18" t="s">
         <v>15</v>
@@ -1793,7 +1801,7 @@
       </c>
       <c r="I18" s="7">
         <f t="shared" si="0"/>
-        <v>56.7</v>
+        <v>63</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>15</v>
@@ -1822,7 +1830,7 @@
       </c>
       <c r="I19" s="7">
         <f t="shared" si="0"/>
-        <v>23.400000000000002</v>
+        <v>26</v>
       </c>
       <c r="J19" s="18" t="s">
         <v>15</v>
@@ -1851,7 +1859,7 @@
       </c>
       <c r="I20" s="7">
         <f t="shared" si="0"/>
-        <v>24.3</v>
+        <v>27</v>
       </c>
       <c r="J20" s="18" t="s">
         <v>15</v>
@@ -1882,7 +1890,7 @@
       </c>
       <c r="I21" s="7">
         <f t="shared" si="0"/>
-        <v>153.9</v>
+        <v>171</v>
       </c>
       <c r="J21" s="18" t="s">
         <v>15</v>
@@ -1913,7 +1921,7 @@
       </c>
       <c r="I22" s="7">
         <f t="shared" si="0"/>
-        <v>131.4</v>
+        <v>146</v>
       </c>
       <c r="J22" s="18" t="s">
         <v>15</v>
@@ -1943,8 +1951,8 @@
         <v>0.24</v>
       </c>
       <c r="I23" s="7">
-        <f t="shared" ref="I23:I43" si="1">H23*$O$2</f>
-        <v>21.599999999999998</v>
+        <f t="shared" ref="I23:I45" si="1">H23*$O$2</f>
+        <v>24</v>
       </c>
       <c r="J23" s="18" t="s">
         <v>15</v>
@@ -1973,7 +1981,7 @@
       </c>
       <c r="I24" s="7">
         <f t="shared" si="1"/>
-        <v>37.799999999999997</v>
+        <v>42</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>15</v>
@@ -2002,7 +2010,7 @@
       </c>
       <c r="I25" s="7">
         <f t="shared" si="1"/>
-        <v>77.400000000000006</v>
+        <v>86</v>
       </c>
       <c r="J25" s="18" t="s">
         <v>15</v>
@@ -2031,7 +2039,7 @@
       </c>
       <c r="I26" s="7">
         <f t="shared" si="1"/>
-        <v>35.1</v>
+        <v>39</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>15</v>
@@ -2060,7 +2068,7 @@
       </c>
       <c r="I27" s="7">
         <f t="shared" si="1"/>
-        <v>58.5</v>
+        <v>65</v>
       </c>
       <c r="J27" s="18" t="s">
         <v>15</v>
@@ -2089,7 +2097,7 @@
       </c>
       <c r="I28" s="7">
         <f t="shared" si="1"/>
-        <v>97.2</v>
+        <v>108</v>
       </c>
       <c r="J28" s="18" t="s">
         <v>15</v>
@@ -2118,7 +2126,7 @@
       </c>
       <c r="I29" s="7">
         <f t="shared" si="1"/>
-        <v>27.9</v>
+        <v>31</v>
       </c>
       <c r="J29" s="18" t="s">
         <v>15</v>
@@ -2126,13 +2134,13 @@
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
-        <v>2012</v>
+        <v>2021</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -2143,11 +2151,11 @@
         <v>59</v>
       </c>
       <c r="H30" s="7">
-        <v>0.15</v>
+        <v>0.34</v>
       </c>
       <c r="I30" s="7">
         <f t="shared" si="1"/>
-        <v>13.5</v>
+        <v>34</v>
       </c>
       <c r="J30" s="18" t="s">
         <v>15</v>
@@ -2155,28 +2163,28 @@
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H31" s="7">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="I31" s="7">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="J31" s="18" t="s">
         <v>15</v>
@@ -2184,7 +2192,7 @@
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <v>2020</v>
+        <v>2000</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>70</v>
@@ -2201,11 +2209,11 @@
         <v>39</v>
       </c>
       <c r="H32" s="7">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="I32" s="7">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f t="shared" ref="I32" si="2">H32*$O$2</f>
+        <v>24</v>
       </c>
       <c r="J32" s="18" t="s">
         <v>15</v>
@@ -2213,7 +2221,7 @@
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>2021</v>
+        <v>2007</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>70</v>
@@ -2230,11 +2238,11 @@
         <v>39</v>
       </c>
       <c r="H33" s="7">
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
       <c r="I33" s="7">
         <f t="shared" si="1"/>
-        <v>21.599999999999998</v>
+        <v>60</v>
       </c>
       <c r="J33" s="18" t="s">
         <v>15</v>
@@ -2242,13 +2250,13 @@
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -2256,14 +2264,14 @@
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H34" s="7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I34" s="7">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="J34" s="18" t="s">
         <v>15</v>
@@ -2271,28 +2279,28 @@
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <v>1993</v>
+        <v>2021</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="H35" s="7">
-        <v>0.15</v>
+        <v>0.24</v>
       </c>
       <c r="I35" s="7">
         <f t="shared" si="1"/>
-        <v>13.5</v>
+        <v>24</v>
       </c>
       <c r="J35" s="18" t="s">
         <v>15</v>
@@ -2300,13 +2308,13 @@
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <v>2002</v>
+        <v>2013</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -2314,14 +2322,14 @@
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="H36" s="7">
-        <v>0.34</v>
+        <v>0.1</v>
       </c>
       <c r="I36" s="7">
         <f t="shared" si="1"/>
-        <v>30.6</v>
+        <v>10</v>
       </c>
       <c r="J36" s="18" t="s">
         <v>15</v>
@@ -2335,7 +2343,7 @@
         <v>78</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -2343,14 +2351,14 @@
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H37" s="7">
-        <v>0.51</v>
+        <v>0.15</v>
       </c>
       <c r="I37" s="7">
         <f t="shared" si="1"/>
-        <v>45.9</v>
+        <v>15</v>
       </c>
       <c r="J37" s="18" t="s">
         <v>15</v>
@@ -2364,7 +2372,7 @@
         <v>78</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2372,14 +2380,14 @@
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H38" s="7">
-        <v>1.03</v>
+        <v>0.34</v>
       </c>
       <c r="I38" s="7">
         <f t="shared" si="1"/>
-        <v>92.7</v>
+        <v>34</v>
       </c>
       <c r="J38" s="18" t="s">
         <v>15</v>
@@ -2387,13 +2395,13 @@
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
-        <v>2004</v>
+        <v>1993</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2401,14 +2409,14 @@
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H39" s="7">
-        <v>0.96</v>
+        <v>0.51</v>
       </c>
       <c r="I39" s="7">
         <f t="shared" si="1"/>
-        <v>86.399999999999991</v>
+        <v>51</v>
       </c>
       <c r="J39" s="18" t="s">
         <v>15</v>
@@ -2416,13 +2424,13 @@
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
-        <v>1993</v>
+        <v>2002</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -2430,14 +2438,14 @@
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H40" s="7">
-        <v>2.3199999999999998</v>
+        <v>1.03</v>
       </c>
       <c r="I40" s="7">
         <f t="shared" si="1"/>
-        <v>208.79999999999998</v>
+        <v>103</v>
       </c>
       <c r="J40" s="18" t="s">
         <v>15</v>
@@ -2445,13 +2453,13 @@
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -2459,14 +2467,14 @@
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="H41" s="7">
-        <v>0.16</v>
+        <v>0.96</v>
       </c>
       <c r="I41" s="7">
         <f t="shared" si="1"/>
-        <v>14.4</v>
+        <v>96</v>
       </c>
       <c r="J41" s="18" t="s">
         <v>15</v>
@@ -2474,13 +2482,13 @@
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
-        <v>2009</v>
+        <v>1993</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -2488,14 +2496,14 @@
         <v>1</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="H42" s="7">
-        <v>0.22</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="I42" s="7">
         <f t="shared" si="1"/>
-        <v>19.8</v>
+        <v>231.99999999999997</v>
       </c>
       <c r="J42" s="18" t="s">
         <v>15</v>
@@ -2503,13 +2511,13 @@
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -2517,14 +2525,14 @@
         <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="H43" s="7">
-        <v>0.44</v>
+        <v>0.16</v>
       </c>
       <c r="I43" s="7">
         <f t="shared" si="1"/>
-        <v>39.6</v>
+        <v>16</v>
       </c>
       <c r="J43" s="18" t="s">
         <v>15</v>
@@ -2532,13 +2540,13 @@
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
-        <v>1996</v>
+        <v>2009</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -2546,14 +2554,14 @@
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="H44" s="7">
-        <v>2.23</v>
+        <v>0.22</v>
       </c>
       <c r="I44" s="7">
-        <f t="shared" ref="I44" si="2">H44*$O$2</f>
-        <v>200.7</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="J44" s="18" t="s">
         <v>15</v>
@@ -2561,13 +2569,13 @@
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
-        <v>1985</v>
+        <v>2007</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -2575,14 +2583,14 @@
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="H45" s="7">
-        <v>0.11</v>
+        <v>0.44</v>
       </c>
       <c r="I45" s="7">
-        <f t="shared" ref="I45" si="3">H45*$O$2</f>
-        <v>9.9</v>
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="J45" s="18" t="s">
         <v>15</v>
@@ -2590,13 +2598,13 @@
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
-        <v>1981</v>
+        <v>1996</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -2604,14 +2612,14 @@
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H46" s="7">
-        <v>0.26</v>
+        <v>2.23</v>
       </c>
       <c r="I46" s="7">
-        <f t="shared" ref="I46" si="4">H46*$O$2</f>
-        <v>23.400000000000002</v>
+        <f t="shared" ref="I46" si="3">H46*$O$2</f>
+        <v>223</v>
       </c>
       <c r="J46" s="18" t="s">
         <v>15</v>
@@ -2619,26 +2627,28 @@
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
-        <v>2005</v>
+        <v>1985</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="8">
         <v>1</v>
       </c>
-      <c r="G47" s="7"/>
+      <c r="G47" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="H47" s="7">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="I47" s="7">
-        <f t="shared" ref="I47" si="5">H47*$O$2</f>
-        <v>4.5</v>
+        <f t="shared" ref="I47" si="4">H47*$O$2</f>
+        <v>11</v>
       </c>
       <c r="J47" s="18" t="s">
         <v>15</v>
@@ -2646,26 +2656,28 @@
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
-        <v>1992</v>
+        <v>1981</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="8">
         <v>1</v>
       </c>
-      <c r="G48" s="7"/>
+      <c r="G48" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="H48" s="7">
-        <v>0.05</v>
+        <v>0.26</v>
       </c>
       <c r="I48" s="7">
-        <f t="shared" ref="I48" si="6">H48*$O$2</f>
-        <v>4.5</v>
+        <f t="shared" ref="I48" si="5">H48*$O$2</f>
+        <v>26</v>
       </c>
       <c r="J48" s="18" t="s">
         <v>15</v>
@@ -2673,13 +2685,13 @@
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <v>1992</v>
+        <v>2005</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -2688,11 +2700,11 @@
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="I49" s="7">
-        <f t="shared" ref="I49" si="7">H49*$O$2</f>
-        <v>7.2</v>
+        <f t="shared" ref="I49" si="6">H49*$O$2</f>
+        <v>5</v>
       </c>
       <c r="J49" s="18" t="s">
         <v>15</v>
@@ -2700,13 +2712,13 @@
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
-        <v>2002</v>
+        <v>1992</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -2718,8 +2730,8 @@
         <v>0.05</v>
       </c>
       <c r="I50" s="7">
-        <f t="shared" ref="I50" si="8">H50*$O$2</f>
-        <v>4.5</v>
+        <f t="shared" ref="I50" si="7">H50*$O$2</f>
+        <v>5</v>
       </c>
       <c r="J50" s="18" t="s">
         <v>15</v>
@@ -2727,28 +2739,82 @@
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
-        <v>2002</v>
+        <v>1992</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="I51" s="7">
+        <f t="shared" ref="I51" si="8">H51*$O$2</f>
+        <v>8</v>
+      </c>
+      <c r="J51" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="4">
+        <v>2002</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="8">
+        <v>1</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="I52" s="7">
+        <f t="shared" ref="I52" si="9">H52*$O$2</f>
+        <v>5</v>
+      </c>
+      <c r="J52" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="4">
+        <v>2002</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="8">
+        <v>2</v>
+      </c>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7">
         <v>0.03</v>
       </c>
-      <c r="I51" s="7">
-        <f t="shared" ref="I51" si="9">H51*$O$2</f>
-        <v>2.6999999999999997</v>
-      </c>
-      <c r="J51" s="18" t="s">
+      <c r="I53" s="7">
+        <f t="shared" ref="I53" si="10">H53*$O$2</f>
+        <v>3</v>
+      </c>
+      <c r="J53" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2762,12 +2828,12 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="F4:F7 F17">
-    <cfRule type="containsText" dxfId="33" priority="97" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="30" priority="99" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F7 F17">
-    <cfRule type="colorScale" priority="98">
+    <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2779,12 +2845,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="29" priority="45" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F24))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2796,11 +2862,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="containsText" dxfId="31" priority="89" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="28" priority="91" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(F8))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="92">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="containsText" dxfId="27" priority="89" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
     <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2812,12 +2895,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="30" priority="87" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F9))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
+  <conditionalFormatting sqref="F10">
+    <cfRule type="containsText" dxfId="26" priority="87" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
     <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2829,12 +2912,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="29" priority="85" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F10))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
+  <conditionalFormatting sqref="F11">
+    <cfRule type="containsText" dxfId="25" priority="85" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
     <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2846,13 +2929,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="28" priority="83" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F11))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="colorScale" priority="84">
+  <conditionalFormatting sqref="F12">
+    <cfRule type="containsText" dxfId="24" priority="79" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2863,12 +2946,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="containsText" dxfId="27" priority="77" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F12))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
+  <conditionalFormatting sqref="F13:F14">
+    <cfRule type="containsText" dxfId="23" priority="77" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:F14">
     <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2880,12 +2963,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13:F14">
-    <cfRule type="containsText" dxfId="26" priority="75" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F13))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13:F14">
+  <conditionalFormatting sqref="F15">
+    <cfRule type="containsText" dxfId="22" priority="75" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2897,12 +2980,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15">
-    <cfRule type="containsText" dxfId="25" priority="73" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15">
+  <conditionalFormatting sqref="F16">
+    <cfRule type="containsText" dxfId="21" priority="73" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
     <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2914,13 +2997,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
-    <cfRule type="containsText" dxfId="24" priority="71" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
-    <cfRule type="colorScale" priority="72">
+  <conditionalFormatting sqref="F18">
+    <cfRule type="containsText" dxfId="20" priority="63" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2931,12 +3014,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
-    <cfRule type="containsText" dxfId="23" priority="61" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
+  <conditionalFormatting sqref="F19">
+    <cfRule type="containsText" dxfId="19" priority="61" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2948,12 +3031,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
-    <cfRule type="containsText" dxfId="22" priority="59" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
+  <conditionalFormatting sqref="F20">
+    <cfRule type="containsText" dxfId="18" priority="59" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2965,12 +3048,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
-    <cfRule type="containsText" dxfId="21" priority="57" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
+  <conditionalFormatting sqref="F21">
+    <cfRule type="containsText" dxfId="17" priority="57" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2982,12 +3065,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
-    <cfRule type="containsText" dxfId="20" priority="55" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F21))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
+  <conditionalFormatting sqref="F22">
+    <cfRule type="containsText" dxfId="16" priority="55" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2999,12 +3082,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="containsText" dxfId="19" priority="53" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
+  <conditionalFormatting sqref="F23">
+    <cfRule type="containsText" dxfId="15" priority="53" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3016,13 +3099,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
-    <cfRule type="containsText" dxfId="18" priority="51" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F23))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
-    <cfRule type="colorScale" priority="52">
+  <conditionalFormatting sqref="F3">
+    <cfRule type="containsText" dxfId="14" priority="41" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -3033,12 +3116,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="containsText" dxfId="17" priority="39" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
+  <conditionalFormatting sqref="F27">
+    <cfRule type="containsText" dxfId="13" priority="35" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="containsText" dxfId="12" priority="39" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3050,12 +3150,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
-    <cfRule type="containsText" dxfId="16" priority="33" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F27))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
+  <conditionalFormatting sqref="F26">
+    <cfRule type="containsText" dxfId="11" priority="37" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F26))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="containsText" dxfId="10" priority="33" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F28))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3067,46 +3184,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25">
-    <cfRule type="containsText" dxfId="15" priority="37" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F25))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
-    <cfRule type="containsText" dxfId="14" priority="35" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F26))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="containsText" dxfId="13" priority="31" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F28))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
+  <conditionalFormatting sqref="F29:F31 F33:F42">
+    <cfRule type="containsText" dxfId="9" priority="31" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:F31 F33:F42">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3118,13 +3201,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F40">
-    <cfRule type="containsText" dxfId="12" priority="29" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F40">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="F43">
+    <cfRule type="containsText" dxfId="8" priority="17" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F43))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -3135,12 +3218,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41">
-    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F41))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F41">
+  <conditionalFormatting sqref="F44:F45">
+    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F44))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:F45">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3152,12 +3235,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F42:F43">
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F42))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F42:F43">
+  <conditionalFormatting sqref="F46:F48">
+    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F46))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:F48">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3169,12 +3252,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F44:F46">
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F44))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:F46">
+  <conditionalFormatting sqref="F49">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F49))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F49">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3186,12 +3269,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F47))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
+  <conditionalFormatting sqref="F50">
+    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F50))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3203,12 +3286,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F48))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
+  <conditionalFormatting sqref="F51">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F51))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3220,12 +3303,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F49))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
+  <conditionalFormatting sqref="F52">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F52))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3237,13 +3320,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F50">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F50))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F50">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="F53">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F53))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F53">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -3254,12 +3337,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(F51))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
+  <conditionalFormatting sqref="F32">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(F32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3297,34 +3380,36 @@
     <hyperlink ref="J27" r:id="rId23" xr:uid="{B8AB633F-C79E-4641-AFB4-7F65634D214B}"/>
     <hyperlink ref="J28" r:id="rId24" xr:uid="{D6CA81C5-FFC1-4861-89D0-3B8270E91B24}"/>
     <hyperlink ref="J29" r:id="rId25" xr:uid="{F029E147-2FC0-4ED4-A9BA-B3AEF8F83338}"/>
-    <hyperlink ref="J30" r:id="rId26" xr:uid="{73A10ED3-2F5B-4F97-81ED-30385FA901D7}"/>
-    <hyperlink ref="J31" r:id="rId27" xr:uid="{40F894A3-654F-48AE-B508-E435F8B7FCC3}"/>
-    <hyperlink ref="J32" r:id="rId28" xr:uid="{26540E1B-8AA5-4119-8344-31C19EC098B6}"/>
-    <hyperlink ref="J33" r:id="rId29" xr:uid="{047833CA-2665-4636-BC0A-889B880D1AC9}"/>
+    <hyperlink ref="J31" r:id="rId26" xr:uid="{73A10ED3-2F5B-4F97-81ED-30385FA901D7}"/>
+    <hyperlink ref="J33" r:id="rId27" xr:uid="{40F894A3-654F-48AE-B508-E435F8B7FCC3}"/>
+    <hyperlink ref="J34" r:id="rId28" xr:uid="{26540E1B-8AA5-4119-8344-31C19EC098B6}"/>
+    <hyperlink ref="J35" r:id="rId29" xr:uid="{047833CA-2665-4636-BC0A-889B880D1AC9}"/>
     <hyperlink ref="J14" r:id="rId30" xr:uid="{D055C12F-058E-42E8-9A2F-4D3F9E4AB17F}"/>
-    <hyperlink ref="J38" r:id="rId31" xr:uid="{DF726C7F-C987-492B-AD45-490E4330D08B}"/>
-    <hyperlink ref="J39" r:id="rId32" xr:uid="{3A3F982A-75C1-43B9-A8FB-651AE97C4F3B}"/>
-    <hyperlink ref="J40" r:id="rId33" xr:uid="{C2C0492D-2383-4293-AA43-769AAF79B00E}"/>
-    <hyperlink ref="J37" r:id="rId34" xr:uid="{A8D496C3-3C82-4BC1-8419-F02CEAAA1708}"/>
-    <hyperlink ref="J36" r:id="rId35" xr:uid="{6F4119D1-AD7B-4530-BC45-0D720C2688AA}"/>
-    <hyperlink ref="J35" r:id="rId36" xr:uid="{EBCE5F45-4195-4D5E-878D-CBF2804B08B4}"/>
-    <hyperlink ref="J34" r:id="rId37" xr:uid="{232755DC-D964-476D-A517-00D6D6DD1904}"/>
+    <hyperlink ref="J40" r:id="rId31" xr:uid="{DF726C7F-C987-492B-AD45-490E4330D08B}"/>
+    <hyperlink ref="J41" r:id="rId32" xr:uid="{3A3F982A-75C1-43B9-A8FB-651AE97C4F3B}"/>
+    <hyperlink ref="J42" r:id="rId33" xr:uid="{C2C0492D-2383-4293-AA43-769AAF79B00E}"/>
+    <hyperlink ref="J39" r:id="rId34" xr:uid="{A8D496C3-3C82-4BC1-8419-F02CEAAA1708}"/>
+    <hyperlink ref="J38" r:id="rId35" xr:uid="{6F4119D1-AD7B-4530-BC45-0D720C2688AA}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{EBCE5F45-4195-4D5E-878D-CBF2804B08B4}"/>
+    <hyperlink ref="J36" r:id="rId37" xr:uid="{232755DC-D964-476D-A517-00D6D6DD1904}"/>
     <hyperlink ref="J7" r:id="rId38" xr:uid="{E4B942A5-8883-4E13-BD74-ABC51325D948}"/>
-    <hyperlink ref="J41" r:id="rId39" xr:uid="{5779549B-DAD5-4010-8F42-12723FFB3FC7}"/>
-    <hyperlink ref="J42" r:id="rId40" xr:uid="{2F4149AC-01D1-4A1E-B537-7EBAC4258E22}"/>
-    <hyperlink ref="J43" r:id="rId41" xr:uid="{94CBABDF-E2E7-4282-9173-12D84F8B6D46}"/>
-    <hyperlink ref="J44" r:id="rId42" xr:uid="{328C6A49-3FE7-4A6E-8FAA-F591F37D4BE5}"/>
-    <hyperlink ref="J45" r:id="rId43" xr:uid="{830C1B92-A98B-4E87-A071-C29E96B7C55E}"/>
-    <hyperlink ref="J46" r:id="rId44" xr:uid="{731AB36A-EB43-4F4D-B942-1D22A7BC4B6B}"/>
-    <hyperlink ref="J47" r:id="rId45" location="price" xr:uid="{B9D8F45C-76AA-4F8B-87FC-AAC293DC68C9}"/>
-    <hyperlink ref="J48" r:id="rId46" xr:uid="{B6EB4A4A-A820-4859-A7A5-B6037A4CB479}"/>
-    <hyperlink ref="J49" r:id="rId47" xr:uid="{EB7AC202-5DAC-4484-8497-F3CC577DED7B}"/>
-    <hyperlink ref="J50" r:id="rId48" xr:uid="{3480EDE6-C77A-4A86-A6AC-8D07EB1A3658}"/>
-    <hyperlink ref="J51" r:id="rId49" xr:uid="{246EE0BE-B71E-448D-BEDD-42B0125A584D}"/>
+    <hyperlink ref="J43" r:id="rId39" xr:uid="{5779549B-DAD5-4010-8F42-12723FFB3FC7}"/>
+    <hyperlink ref="J44" r:id="rId40" xr:uid="{2F4149AC-01D1-4A1E-B537-7EBAC4258E22}"/>
+    <hyperlink ref="J45" r:id="rId41" xr:uid="{94CBABDF-E2E7-4282-9173-12D84F8B6D46}"/>
+    <hyperlink ref="J46" r:id="rId42" xr:uid="{328C6A49-3FE7-4A6E-8FAA-F591F37D4BE5}"/>
+    <hyperlink ref="J47" r:id="rId43" xr:uid="{830C1B92-A98B-4E87-A071-C29E96B7C55E}"/>
+    <hyperlink ref="J48" r:id="rId44" xr:uid="{731AB36A-EB43-4F4D-B942-1D22A7BC4B6B}"/>
+    <hyperlink ref="J49" r:id="rId45" location="price" xr:uid="{B9D8F45C-76AA-4F8B-87FC-AAC293DC68C9}"/>
+    <hyperlink ref="J50" r:id="rId46" xr:uid="{B6EB4A4A-A820-4859-A7A5-B6037A4CB479}"/>
+    <hyperlink ref="J51" r:id="rId47" xr:uid="{EB7AC202-5DAC-4484-8497-F3CC577DED7B}"/>
+    <hyperlink ref="J52" r:id="rId48" xr:uid="{3480EDE6-C77A-4A86-A6AC-8D07EB1A3658}"/>
+    <hyperlink ref="J53" r:id="rId49" xr:uid="{246EE0BE-B71E-448D-BEDD-42B0125A584D}"/>
+    <hyperlink ref="J30" r:id="rId50" xr:uid="{F92A4148-4754-431F-993D-E00DDB823E84}"/>
+    <hyperlink ref="J32" r:id="rId51" xr:uid="{FBC9555C-B864-4E82-926A-09CDCE70881B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId50"/>
-  <legacyDrawing r:id="rId51"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId52"/>
+  <legacyDrawing r:id="rId53"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
& - 81457882 от 11.09.2025 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/Foreign_various/Foreighn_duplicates.xlsx
+++ b/Collections/Foreign_various/Foreighn_duplicates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\Foreign_various\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E881BADA-0527-46E3-A7C1-07E4907C3411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B19A9-2E61-4AD5-96B1-E9CFC3156A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Links" sheetId="13" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Монеты!$A$2:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Монеты!$A$2:$E$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,6 +29,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -95,9 +98,6 @@
     <t>Штук</t>
   </si>
   <si>
-    <t>Цена</t>
-  </si>
-  <si>
     <t>Страна</t>
   </si>
   <si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Subtype_1#Value</t>
+  </si>
+  <si>
+    <t>Цена, ориентировочно</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1288,7 @@
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1313,47 +1316,47 @@
         <v>10</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="I1" s="31"/>
       <c r="J1" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>
       <c r="B2" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>104</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>71</v>
       </c>
       <c r="J2" s="26"/>
       <c r="K2" s="1"/>
       <c r="O2" s="6">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1361,30 +1364,30 @@
         <v>2015</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="8">
         <v>5</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="7">
         <v>0.26</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" ref="I3:I22" si="0">H3*$O$2</f>
-        <v>26</v>
+        <v>21.32</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -1393,10 +1396,10 @@
         <v>2015</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1404,17 +1407,17 @@
         <v>2</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="7">
         <v>0.63</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>51.660000000000004</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1422,10 +1425,10 @@
         <v>2016</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1433,17 +1436,17 @@
         <v>2</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7">
         <v>0.94</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>77.08</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1451,10 +1454,10 @@
         <v>2015</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1462,17 +1465,17 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="7">
         <v>1.1000000000000001</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="0"/>
-        <v>110.00000000000001</v>
+        <v>90.2</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1480,10 +1483,10 @@
         <v>2005</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1491,17 +1494,17 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="7">
         <v>1.06</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="0"/>
-        <v>106</v>
+        <v>86.92</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1509,10 +1512,10 @@
         <v>2000</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1520,17 +1523,17 @@
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="7">
         <v>0.36</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>29.52</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1538,10 +1541,10 @@
         <v>2015</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1549,17 +1552,17 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="7">
         <v>0.49</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>40.18</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1567,10 +1570,10 @@
         <v>2012</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1578,17 +1581,17 @@
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="7">
         <v>1.1399999999999999</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="0"/>
-        <v>113.99999999999999</v>
+        <v>93.47999999999999</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1596,10 +1599,10 @@
         <v>1996</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1607,17 +1610,17 @@
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="7">
         <v>0.39</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>31.98</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1625,10 +1628,10 @@
         <v>1996</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1636,17 +1639,17 @@
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="7">
         <v>0.39</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>31.98</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1654,10 +1657,10 @@
         <v>2009</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1665,17 +1668,17 @@
         <v>2</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="7">
         <v>0.13</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>10.66</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1683,10 +1686,10 @@
         <v>2009</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1694,17 +1697,17 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H14" s="7">
         <v>0.16</v>
       </c>
       <c r="I14" s="7">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>13.120000000000001</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1712,10 +1715,10 @@
         <v>1995</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1723,17 +1726,17 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H15" s="7">
         <v>0.22</v>
       </c>
       <c r="I15" s="7">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>18.04</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1741,10 +1744,10 @@
         <v>1999</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1752,17 +1755,17 @@
         <v>2</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" s="7">
         <v>0.22</v>
       </c>
       <c r="I16" s="7">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>18.04</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1770,10 +1773,10 @@
         <v>1987</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1781,17 +1784,17 @@
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" s="7">
         <v>0.3</v>
       </c>
       <c r="I17" s="7">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>24.599999999999998</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1799,10 +1802,10 @@
         <v>2012</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1810,17 +1813,17 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H18" s="7">
         <v>0.63</v>
       </c>
       <c r="I18" s="7">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>51.660000000000004</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1828,10 +1831,10 @@
         <v>2009</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1839,17 +1842,17 @@
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" s="7">
         <v>0.26</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>21.32</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1857,10 +1860,10 @@
         <v>1996</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1868,17 +1871,17 @@
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H20" s="7">
         <v>0.27</v>
       </c>
       <c r="I20" s="7">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>22.14</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1886,10 +1889,10 @@
         <v>2001</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="19">
         <v>2544</v>
@@ -1899,17 +1902,17 @@
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="7">
         <v>1.71</v>
       </c>
       <c r="I21" s="7">
         <f t="shared" si="0"/>
-        <v>171</v>
+        <v>140.22</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1917,10 +1920,10 @@
         <v>1990</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="19">
         <v>2533</v>
@@ -1930,17 +1933,17 @@
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="7">
         <v>1.46</v>
       </c>
       <c r="I22" s="7">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>119.72</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1948,30 +1951,30 @@
         <v>2013</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="8">
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H23" s="7">
         <v>0.24</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" ref="I23:I45" si="1">H23*$O$2</f>
-        <v>24</v>
+        <v>19.68</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1979,10 +1982,10 @@
         <v>2003</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1990,17 +1993,17 @@
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H24" s="7">
         <v>0.42</v>
       </c>
       <c r="I24" s="7">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>34.44</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2008,10 +2011,10 @@
         <v>2016</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -2019,17 +2022,17 @@
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H25" s="7">
         <v>0.86</v>
       </c>
       <c r="I25" s="7">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>70.52</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2037,10 +2040,10 @@
         <v>2014</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -2048,17 +2051,17 @@
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H26" s="7">
         <v>0.39</v>
       </c>
       <c r="I26" s="7">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>31.98</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2066,10 +2069,10 @@
         <v>2014</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -2077,17 +2080,17 @@
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" s="7">
         <v>0.65</v>
       </c>
       <c r="I27" s="7">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>53.300000000000004</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2095,10 +2098,10 @@
         <v>2018</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -2106,17 +2109,17 @@
         <v>1</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H28" s="7">
         <v>1.08</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>88.56</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2124,10 +2127,10 @@
         <v>2009</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -2135,17 +2138,17 @@
         <v>1</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H29" s="7">
         <v>0.31</v>
       </c>
       <c r="I29" s="7">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>25.419999999999998</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2153,10 +2156,10 @@
         <v>2021</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -2164,17 +2167,17 @@
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H30" s="7">
         <v>0.34</v>
       </c>
       <c r="I30" s="7">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>27.880000000000003</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2182,10 +2185,10 @@
         <v>2012</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -2193,17 +2196,17 @@
         <v>2</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H31" s="7">
         <v>0.15</v>
       </c>
       <c r="I31" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.299999999999999</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2211,10 +2214,10 @@
         <v>2000</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -2222,17 +2225,17 @@
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H32" s="7">
         <v>0.24</v>
       </c>
       <c r="I32" s="7">
         <f t="shared" ref="I32" si="2">H32*$O$2</f>
-        <v>24</v>
+        <v>19.68</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2240,10 +2243,10 @@
         <v>2007</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -2251,17 +2254,17 @@
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H33" s="7">
         <v>0.6</v>
       </c>
       <c r="I33" s="7">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>49.199999999999996</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2269,10 +2272,10 @@
         <v>2020</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -2280,17 +2283,17 @@
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H34" s="7">
         <v>0.3</v>
       </c>
       <c r="I34" s="7">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>24.599999999999998</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2298,10 +2301,10 @@
         <v>2021</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -2309,17 +2312,17 @@
         <v>2</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H35" s="7">
         <v>0.24</v>
       </c>
       <c r="I35" s="7">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>19.68</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2327,10 +2330,10 @@
         <v>2013</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -2338,17 +2341,17 @@
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H36" s="7">
         <v>0.1</v>
       </c>
       <c r="I36" s="7">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8.2000000000000011</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2356,10 +2359,10 @@
         <v>1993</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -2367,17 +2370,17 @@
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H37" s="7">
         <v>0.15</v>
       </c>
       <c r="I37" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.299999999999999</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2385,10 +2388,10 @@
         <v>2002</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2396,17 +2399,17 @@
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H38" s="7">
         <v>0.34</v>
       </c>
       <c r="I38" s="7">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>27.880000000000003</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2414,10 +2417,10 @@
         <v>1993</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2425,17 +2428,17 @@
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H39" s="7">
         <v>0.51</v>
       </c>
       <c r="I39" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>41.82</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2443,10 +2446,10 @@
         <v>2002</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -2454,17 +2457,17 @@
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H40" s="7">
         <v>1.03</v>
       </c>
       <c r="I40" s="7">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>84.460000000000008</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2472,10 +2475,10 @@
         <v>2004</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -2483,17 +2486,17 @@
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H41" s="7">
         <v>0.96</v>
       </c>
       <c r="I41" s="7">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>78.72</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2501,10 +2504,10 @@
         <v>1993</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -2512,17 +2515,17 @@
         <v>1</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H42" s="7">
         <v>2.3199999999999998</v>
       </c>
       <c r="I42" s="7">
         <f t="shared" si="1"/>
-        <v>231.99999999999997</v>
+        <v>190.23999999999998</v>
       </c>
       <c r="J42" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2530,10 +2533,10 @@
         <v>2006</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -2541,17 +2544,17 @@
         <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H43" s="7">
         <v>0.16</v>
       </c>
       <c r="I43" s="7">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>13.120000000000001</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2559,10 +2562,10 @@
         <v>2009</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -2570,17 +2573,17 @@
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H44" s="7">
         <v>0.22</v>
       </c>
       <c r="I44" s="7">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>18.04</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2588,10 +2591,10 @@
         <v>2007</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -2599,17 +2602,17 @@
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H45" s="7">
         <v>0.44</v>
       </c>
       <c r="I45" s="7">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>36.08</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2617,10 +2620,10 @@
         <v>1996</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -2628,17 +2631,17 @@
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H46" s="7">
         <v>2.23</v>
       </c>
       <c r="I46" s="7">
         <f t="shared" ref="I46" si="3">H46*$O$2</f>
-        <v>223</v>
+        <v>182.85999999999999</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2646,10 +2649,10 @@
         <v>1985</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -2657,17 +2660,17 @@
         <v>1</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H47" s="7">
         <v>0.11</v>
       </c>
       <c r="I47" s="7">
         <f t="shared" ref="I47" si="4">H47*$O$2</f>
-        <v>11</v>
+        <v>9.02</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2675,10 +2678,10 @@
         <v>1981</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -2686,17 +2689,17 @@
         <v>1</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H48" s="7">
         <v>0.26</v>
       </c>
       <c r="I48" s="7">
         <f t="shared" ref="I48" si="5">H48*$O$2</f>
-        <v>26</v>
+        <v>21.32</v>
       </c>
       <c r="J48" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2704,10 +2707,10 @@
         <v>2005</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -2720,10 +2723,10 @@
       </c>
       <c r="I49" s="7">
         <f t="shared" ref="I49" si="6">H49*$O$2</f>
-        <v>5</v>
+        <v>4.1000000000000005</v>
       </c>
       <c r="J49" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2731,10 +2734,10 @@
         <v>1992</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -2747,10 +2750,10 @@
       </c>
       <c r="I50" s="7">
         <f t="shared" ref="I50" si="7">H50*$O$2</f>
-        <v>5</v>
+        <v>4.1000000000000005</v>
       </c>
       <c r="J50" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2758,10 +2761,10 @@
         <v>1992</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -2774,10 +2777,10 @@
       </c>
       <c r="I51" s="7">
         <f t="shared" ref="I51" si="8">H51*$O$2</f>
-        <v>8</v>
+        <v>6.5600000000000005</v>
       </c>
       <c r="J51" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2785,10 +2788,10 @@
         <v>2002</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -2801,10 +2804,10 @@
       </c>
       <c r="I52" s="7">
         <f t="shared" ref="I52" si="9">H52*$O$2</f>
-        <v>5</v>
+        <v>4.1000000000000005</v>
       </c>
       <c r="J52" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2812,10 +2815,10 @@
         <v>2002</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -2828,14 +2831,14 @@
       </c>
       <c r="I53" s="7">
         <f t="shared" ref="I53" si="10">H53*$O$2</f>
-        <v>3</v>
+        <v>2.46</v>
       </c>
       <c r="J53" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E2" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A2:E53" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="C1:E1"/>

</xml_diff>